<commit_message>
added elevation and latitude spreadsheet
</commit_message>
<xml_diff>
--- a/Rana and Lithobates spreadsheet.xlsx
+++ b/Rana and Lithobates spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c678cee08d214e79/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tito/fr10_evolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB927D87-73D9-FA4C-B48E-99C2616DA4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C339D5FD-DAF0-6F49-91C0-995306A89A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BFB6A9C7-1922-C24B-BC94-9639BD1A821B}"/>
+    <workbookView xWindow="2320" yWindow="1420" windowWidth="28800" windowHeight="16340" xr2:uid="{BFB6A9C7-1922-C24B-BC94-9639BD1A821B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="166">
   <si>
     <t>Genus</t>
   </si>
@@ -284,78 +284,30 @@
     <t>0-701 m</t>
   </si>
   <si>
-    <t>Maximum Decimal Latitude</t>
-  </si>
-  <si>
     <t>800-2740 m</t>
   </si>
   <si>
     <t>2740 m</t>
   </si>
   <si>
-    <t>Chalcoran</t>
-  </si>
-  <si>
     <t>chalconota</t>
   </si>
   <si>
     <t>1571 m</t>
   </si>
   <si>
-    <t>see level-1950</t>
-  </si>
-  <si>
-    <t>"-0.7166666667 36.6500000000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	41.2875111111 -124.0825055556</t>
-  </si>
-  <si>
-    <t>14.44 108.3827778</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 	33.15468 -115.45084</t>
-  </si>
-  <si>
-    <t>43.6906773056 -122.0292366389</t>
-  </si>
-  <si>
-    <t>32.35222 -84.96889</t>
-  </si>
-  <si>
-    <t>43362 -74.587</t>
-  </si>
-  <si>
-    <t>7.9 98.31667</t>
-  </si>
-  <si>
     <t xml:space="preserve">900 m </t>
   </si>
   <si>
     <t xml:space="preserve">1200 m </t>
   </si>
   <si>
-    <t>9.3978333333 -0.9843333333</t>
-  </si>
-  <si>
-    <t>25.7609 -80.5922</t>
-  </si>
-  <si>
     <t>200-1600 m</t>
   </si>
   <si>
     <t>1600 m</t>
   </si>
   <si>
-    <t xml:space="preserve">	21.5646944444 93.9732222222</t>
-  </si>
-  <si>
-    <t>27.7487300000 98.3491200000</t>
-  </si>
-  <si>
-    <t>33.8085972222 -116.7247777778</t>
-  </si>
-  <si>
     <t xml:space="preserve">90-105 m </t>
   </si>
   <si>
@@ -365,33 +317,18 @@
     <t>nazgul</t>
   </si>
   <si>
-    <t>19.7001 104.7381</t>
-  </si>
-  <si>
     <t>914-1219 m</t>
   </si>
   <si>
     <t>1219 m</t>
   </si>
   <si>
-    <t>9.0462694444 125.7010000000</t>
-  </si>
-  <si>
-    <t>12.4341 99.1451</t>
-  </si>
-  <si>
     <t>130 m</t>
   </si>
   <si>
-    <t>28.23795 107.15440</t>
-  </si>
-  <si>
     <t>orphnocnemis</t>
   </si>
   <si>
-    <t>"-6.8845914 134.2601762"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +1500 m</t>
   </si>
   <si>
@@ -401,74 +338,274 @@
     <t xml:space="preserve">sea level- 3352 m </t>
   </si>
   <si>
-    <t>39.4746017 -80.8636016</t>
-  </si>
-  <si>
-    <t>22.7318570 101.0742187</t>
-  </si>
-  <si>
     <t>1150-2300 m</t>
   </si>
   <si>
     <t>2300 m</t>
   </si>
   <si>
-    <t>42.68247546904018 -0.5398365228637998</t>
-  </si>
-  <si>
     <t xml:space="preserve">300-1600 m </t>
   </si>
   <si>
-    <t>28.1 117.43333</t>
-  </si>
-  <si>
-    <t>31.7285 48.7215</t>
-  </si>
-  <si>
-    <t>34.98333 135.82486</t>
-  </si>
-  <si>
     <t>near sea level- 1100 m</t>
   </si>
   <si>
     <t>1100 m</t>
   </si>
   <si>
-    <t>9.434116 118.389104</t>
-  </si>
-  <si>
-    <t>38.33346 -119.640055</t>
-  </si>
-  <si>
-    <t>36.8 -76.1</t>
-  </si>
-  <si>
-    <t>"-3.42398 102.262065"</t>
-  </si>
-  <si>
     <t>1220 m</t>
   </si>
   <si>
     <t>sylvatica</t>
   </si>
   <si>
-    <t>59.4197270000 -136.0662850000</t>
-  </si>
-  <si>
-    <t>35.47014 139.01167</t>
-  </si>
-  <si>
     <t>sea level- 2000 meters</t>
   </si>
   <si>
-    <t>China, japan, germany, norway, korea</t>
+    <t>CT max</t>
+  </si>
+  <si>
+    <t>CT min</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>25ºC (In tadpoles)</t>
+  </si>
+  <si>
+    <t>32ºC (In tadpoles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4000 m </t>
+  </si>
+  <si>
+    <r>
+      <t>Navas, C. A., Gomes, F. R., &amp; Carvalho, J. E. (2008). Thermal relationships and exercise physiology in anuran amphibians: integration and evolutionary implications. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Comparative Biochemistry and Physiology Part A: Molecular &amp; Integrative Physiology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>151</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3), 344-362.</t>
+    </r>
+  </si>
+  <si>
+    <t>Chalcorana</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>33ºC</t>
+  </si>
+  <si>
+    <r>
+      <t>Fontaine, S. S., Mineo, P. M., &amp; Kohl, K. D. (2021). Experimental depletion of gut microbiota diversity reduces host thermal tolerance and fitness under heat stress in a vertebrate ectotherm. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bioRxiv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 2021-06.</t>
+    </r>
+  </si>
+  <si>
+    <t>sea level-1950</t>
+  </si>
+  <si>
+    <t>sea level - 1000</t>
+  </si>
+  <si>
+    <t>0-1000</t>
+  </si>
+  <si>
+    <t>1200-1800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-150 m </t>
+  </si>
+  <si>
+    <t>0-1500 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500-1500 m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-1571 m </t>
+  </si>
+  <si>
+    <t>0-200 m</t>
+  </si>
+  <si>
+    <t>1500-4000 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-600 m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-300 m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">800- 2500 m </t>
+  </si>
+  <si>
+    <t>19.436500 / 49.253597</t>
+  </si>
+  <si>
+    <t>45-1954 m</t>
+  </si>
+  <si>
+    <t>22.838833 / 33.831988</t>
+  </si>
+  <si>
+    <t>"-28.074833 / -0.976667"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"34.879516 / 57.890000" </t>
+  </si>
+  <si>
+    <t>"14.341389 / 14.444167"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	"14.984200 / 33.797955"</t>
+  </si>
+  <si>
+    <t>"27.762700 / 30.693197"</t>
+  </si>
+  <si>
+    <t>"8.378183 / 10.574833"</t>
+  </si>
+  <si>
+    <t>"22.315556 / 22.349444"</t>
+  </si>
+  <si>
+    <t>"29.642430 / 49.171196"</t>
+  </si>
+  <si>
+    <t>"-3.299040 / 25.559278"</t>
+  </si>
+  <si>
+    <t>"-8.500000 / 9.259710</t>
+  </si>
+  <si>
+    <t>"26.262150 / 30.671284"</t>
+  </si>
+  <si>
+    <t>"21.172750 / 25.317778"</t>
+  </si>
+  <si>
+    <t>"-8.438097 / 27.613139"</t>
+  </si>
+  <si>
+    <t>"27.74873"</t>
+  </si>
+  <si>
+    <t>"33.779590 / 40.200500</t>
+  </si>
+  <si>
+    <t>"18.725333 / 27.611972"</t>
+  </si>
+  <si>
+    <t>"8.41900 / 12.05262"</t>
+  </si>
+  <si>
+    <t>"8.378183 / 26.714472"</t>
+  </si>
+  <si>
+    <t>"29.16778"</t>
+  </si>
+  <si>
+    <t>"-10.03940 / -3.36700"</t>
+  </si>
+  <si>
+    <t>"9.730430 / 60.006020"</t>
+  </si>
+  <si>
+    <t>"22.731857 / 25.870056"</t>
+  </si>
+  <si>
+    <t>"22.333333"</t>
+  </si>
+  <si>
+    <t>"55.7047"</t>
+  </si>
+  <si>
+    <t>"20.6670 / 22.1329"</t>
+  </si>
+  <si>
+    <t>"37.662850 / 40.254472"</t>
+  </si>
+  <si>
+    <t>"24.705542 / 39.646830"</t>
+  </si>
+  <si>
+    <t>"--3.42398 / 3.33289"</t>
+  </si>
+  <si>
+    <t>"36.638000 / 64.912244"</t>
+  </si>
+  <si>
+    <t>"51.62954 / 58.38630"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,6 +617,25 @@
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -503,10 +659,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,18 +689,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F791CAA-1F25-514D-A131-A2C30660A13C}" name="Table2" displayName="Table2" ref="C4:H45" totalsRowShown="0">
-  <autoFilter ref="C4:H45" xr:uid="{3F791CAA-1F25-514D-A131-A2C30660A13C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:H45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F791CAA-1F25-514D-A131-A2C30660A13C}" name="Table2" displayName="Table2" ref="C4:J45" totalsRowShown="0">
+  <autoFilter ref="C4:J45" xr:uid="{3F791CAA-1F25-514D-A131-A2C30660A13C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:I45">
     <sortCondition ref="D5:D45"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{85BB24E2-2F79-E94C-A0A2-1E284DAB1715}" name="Genus"/>
     <tableColumn id="2" xr3:uid="{18EA0803-0C32-724C-8568-72741729C42D}" name="Species"/>
     <tableColumn id="3" xr3:uid="{77ABCC53-DDC1-674C-A79B-EB0250C943E4}" name="Latitudinal Range"/>
-    <tableColumn id="4" xr3:uid="{6F6BC9CD-586A-D443-9921-797F5F187893}" name="Maximum Decimal Latitude"/>
     <tableColumn id="5" xr3:uid="{174D935F-A796-EC4A-83AC-659883B3E12F}" name="Elevation Range"/>
+    <tableColumn id="8" xr3:uid="{237BB69C-6221-0241-9E08-58C71285F43C}" name="CT max"/>
+    <tableColumn id="9" xr3:uid="{C5D53F3E-2929-0641-8DDD-0A973290B3F5}" name="CT min"/>
     <tableColumn id="6" xr3:uid="{DFF076DB-9147-B04B-B949-8BEB61F38F74}" name="Max Elevation"/>
+    <tableColumn id="12" xr3:uid="{4B3D0D43-F50B-0D40-96F9-DD42DF66F0AD}" name="Sources"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -843,24 +1005,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231ACA80-9D1C-0943-9754-9D2A8B05A301}">
-  <dimension ref="C4:H45"/>
+  <dimension ref="C4:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="38" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="48.5" customWidth="1"/>
+    <col min="6" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="42.5" customWidth="1"/>
+    <col min="10" max="10" width="60.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -871,27 +1033,40 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="H4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
+      <c r="E5" t="str">
+        <f>"-4.711028 / 11.307222"</f>
+        <v>-4.711028 / 11.307222</v>
+      </c>
+      <c r="F5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -899,11 +1074,13 @@
         <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+      <c r="F6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -911,14 +1088,13 @@
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>20</v>
       </c>
@@ -926,11 +1102,13 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="F8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -938,14 +1116,13 @@
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>57</v>
       </c>
@@ -953,11 +1130,13 @@
         <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>7</v>
       </c>
@@ -965,43 +1144,88 @@
         <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" t="s">
         <v>83</v>
       </c>
-      <c r="H11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="3:10" ht="17" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" t="s">
         <v>85</v>
       </c>
-      <c r="D13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>57</v>
       </c>
@@ -1009,13 +1233,19 @@
         <v>58</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>95</v>
+        <v>143</v>
+      </c>
+      <c r="F15" t="s">
+        <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" ht="18" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>28</v>
       </c>
@@ -1023,13 +1253,22 @@
         <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>96</v>
+        <v>144</v>
+      </c>
+      <c r="F16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" t="s">
+        <v>117</v>
       </c>
       <c r="H16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="I16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>28</v>
       </c>
@@ -1037,24 +1276,30 @@
         <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="F17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>57</v>
       </c>
       <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E18" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>42</v>
       </c>
@@ -1062,38 +1307,47 @@
         <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="G20" t="s">
+      <c r="E20">
+        <v>32.878729999999997</v>
+      </c>
+      <c r="F20" t="s">
         <v>60</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>18</v>
       </c>
@@ -1101,24 +1355,30 @@
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" t="s">
         <v>76</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>23</v>
       </c>
       <c r="D23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>7</v>
       </c>
@@ -1126,30 +1386,33 @@
         <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" t="s">
         <v>64</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" t="s">
-        <v>106</v>
-      </c>
-      <c r="H25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="E25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>20</v>
       </c>
@@ -1157,16 +1420,16 @@
         <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G26" t="s">
-        <v>110</v>
-      </c>
-      <c r="H26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="F26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>13</v>
       </c>
@@ -1174,16 +1437,16 @@
         <v>14</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" t="s">
         <v>70</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>28</v>
       </c>
@@ -1191,13 +1454,13 @@
         <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>5</v>
       </c>
@@ -1205,30 +1468,33 @@
         <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G29" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" t="s">
         <v>67</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
-      </c>
-      <c r="G30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" t="s">
         <v>72</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>55</v>
       </c>
@@ -1236,24 +1502,33 @@
         <v>53</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="F31" t="s">
+        <v>125</v>
+      </c>
+      <c r="I31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>51</v>
       </c>
       <c r="D32" t="s">
         <v>52</v>
       </c>
-      <c r="H32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="E32" s="6">
+        <v>4.3369999999999997</v>
+      </c>
+      <c r="F32" t="s">
+        <v>125</v>
+      </c>
+      <c r="I32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>46</v>
       </c>
@@ -1261,16 +1536,16 @@
         <v>45</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="F33" t="s">
+        <v>99</v>
+      </c>
+      <c r="I33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>47</v>
       </c>
@@ -1278,33 +1553,33 @@
         <v>38</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G34" t="s">
-        <v>123</v>
-      </c>
-      <c r="H34" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="F34" t="s">
+        <v>100</v>
+      </c>
+      <c r="I34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
-      <c r="E35" t="s">
-        <v>125</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="E35" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" t="s">
         <v>62</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>18</v>
       </c>
@@ -1312,16 +1587,16 @@
         <v>37</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G36" t="s">
-        <v>126</v>
-      </c>
-      <c r="H36" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>16</v>
       </c>
@@ -1329,16 +1604,16 @@
         <v>17</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G37" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37" t="s">
         <v>74</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>40</v>
       </c>
@@ -1346,27 +1621,30 @@
         <v>39</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G38" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="F38" t="s">
+        <v>103</v>
+      </c>
+      <c r="I38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>50</v>
       </c>
       <c r="D39" t="s">
         <v>49</v>
       </c>
-      <c r="E39" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="E39" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>7</v>
       </c>
@@ -1374,16 +1652,16 @@
         <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G40" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" t="s">
         <v>66</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>7</v>
       </c>
@@ -1391,10 +1669,13 @@
         <v>44</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+      <c r="F41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>35</v>
       </c>
@@ -1402,24 +1683,27 @@
         <v>36</v>
       </c>
       <c r="E42" t="s">
-        <v>135</v>
-      </c>
-      <c r="H42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="F42" t="s">
+        <v>132</v>
+      </c>
+      <c r="I42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8" ht="18" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" ht="18" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>5</v>
       </c>
@@ -1427,16 +1711,16 @@
         <v>12</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G44" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44" t="s">
         <v>68</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>5</v>
       </c>
@@ -1444,16 +1728,17 @@
         <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>141</v>
-      </c>
-      <c r="G45" t="s">
-        <v>140</v>
-      </c>
-      <c r="H45" t="s">
+        <v>165</v>
+      </c>
+      <c r="F45" t="s">
+        <v>107</v>
+      </c>
+      <c r="I45" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">

</xml_diff>